<commit_message>
validator and static page created
</commit_message>
<xml_diff>
--- a/public/exportdata.xlsx
+++ b/public/exportdata.xlsx
@@ -451,7 +451,7 @@
         <v>Hojiakbar Rayimberdiyev</v>
       </c>
       <c r="C2">
-        <v>888323345454</v>
+        <v>885557777</v>
       </c>
       <c r="D2" t="str">
         <v>Xorazm Xonqa Amudaryo Saxiylar28</v>
@@ -478,7 +478,7 @@
         <v>2023-01-26T11:35:36.674Z</v>
       </c>
       <c r="L2" t="str">
-        <v>2023-01-26T11:35:36.674Z</v>
+        <v>2023-01-29T12:12:02.404Z</v>
       </c>
       <c r="M2">
         <v>0</v>

</xml_diff>